<commit_message>
Added more info on Task List.xlsx
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Start Menu Scene" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
   <si>
     <t>In progress</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Sword Follows Mouse</t>
+  </si>
+  <si>
+    <t>Has 3 Health</t>
+  </si>
+  <si>
+    <t>Breaks</t>
   </si>
 </sst>
 </file>
@@ -659,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -904,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,207 +1290,221 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>56</v>
+      <c r="A58" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B79" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B88" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B94" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B95" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B98" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B100" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B106" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1892,6 +1912,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0C5AAC1B3A5834698B991C8B7BE0A43" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d8bfae07456ed53bf096f88a87e9c3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c372ca1-4d00-4da0-9d60-1d24f5b7546b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3317282adf720fe49703ecb68c6f20" ns2:_="">
     <xsd:import namespace="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -2037,12 +2063,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2053,6 +2073,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D8B4A51-A72D-4F05-84AE-D0EEBFFC2F6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2070,22 +2106,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed Sprites + Edited Task List.xlsx
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11490" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="Start Menu Scene" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="100">
   <si>
     <t>In progress</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Sign-Off</t>
   </si>
   <si>
-    <t xml:space="preserve">Committed </t>
-  </si>
-  <si>
     <t>Asset</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Not Started/Assigned To</t>
-  </si>
-  <si>
     <t>Fly</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>Wings</t>
   </si>
   <si>
-    <t>Eyes?</t>
-  </si>
-  <si>
     <t>Fly in "Circle"</t>
   </si>
   <si>
@@ -300,6 +291,45 @@
   </si>
   <si>
     <t>Breaks</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>enemyfly</t>
+  </si>
+  <si>
+    <t>Prefab</t>
+  </si>
+  <si>
+    <t>enemyFly</t>
+  </si>
+  <si>
+    <t>Cj</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Octavio</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>(Already Implemented)</t>
+  </si>
+  <si>
+    <t>Found Correct Version (If Applicable)</t>
+  </si>
+  <si>
+    <t>Ready to be Implemented</t>
+  </si>
+  <si>
+    <t>Olivia &amp; Octavio</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -665,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,16 +716,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -706,7 +736,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -721,10 +751,14 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -732,9 +766,11 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -742,9 +778,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -764,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -786,10 +820,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -803,7 +841,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -813,7 +851,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -830,10 +868,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -843,9 +881,11 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -853,9 +893,11 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -863,9 +905,11 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -873,33 +917,63 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,16 +1007,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -968,44 +1042,68 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
@@ -1024,8 +1122,9 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1035,18 +1134,20 @@
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1065,8 +1166,15 @@
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -1074,29 +1182,47 @@
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
@@ -1111,7 +1237,12 @@
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1119,12 +1250,12 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1135,20 +1266,25 @@
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1158,24 +1294,28 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>26</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>27</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
@@ -1185,321 +1325,464 @@
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>58</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C90" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B96" t="s">
+        <v>61</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>62</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>63</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" t="s">
+        <v>94</v>
+      </c>
+      <c r="D100" t="s">
+        <v>94</v>
+      </c>
+      <c r="E100" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>31</v>
       </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B67" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B105" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="C106" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B79" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B88" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B94" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B98" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B103" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B106" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" t="s">
-        <v>79</v>
+      <c r="B108" t="s">
+        <v>75</v>
+      </c>
+      <c r="C108" t="s">
+        <v>94</v>
+      </c>
+      <c r="D108" t="s">
+        <v>94</v>
+      </c>
+      <c r="E108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" t="s">
+        <v>76</v>
+      </c>
+      <c r="C109" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" t="s">
+        <v>94</v>
+      </c>
+      <c r="E109" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1513,7 +1796,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,16 +1816,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1553,22 +1836,28 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1584,29 +1873,42 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1614,8 +1916,12 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1623,13 +1929,6 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1714,7 +2013,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,16 +2033,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1754,10 +2053,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1765,7 +2067,10 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1786,24 +2091,36 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
@@ -1817,10 +2134,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1912,9 +2229,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2064,26 +2384,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2107,9 +2416,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>